<commit_message>
Initial commit: added all projects + readmes (media coming later)
</commit_message>
<xml_diff>
--- a/docs/essence-originals-projects.xlsx
+++ b/docs/essence-originals-projects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\electric-essence\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFA5D6A-AA5D-435F-8334-E2858EDF896A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C10AC78-D2D3-4E99-9BED-941BBD92DFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C837B0F8-5954-4C5E-A065-EBAD09D629A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{C837B0F8-5954-4C5E-A065-EBAD09D629A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -45,15 +45,9 @@
     <t>3 Versions</t>
   </si>
   <si>
-    <t>• Memory LED</t>
-  </si>
-  <si>
     <t>• Shadow Memory</t>
   </si>
   <si>
-    <t>• Memory Bloom</t>
-  </si>
-  <si>
     <t>LED glows peacefully when idle, becomes disturbed when button pressed.</t>
   </si>
   <si>
@@ -67,6 +61,12 @@
   </si>
   <si>
     <t>An LED stays  on after detecting sound in the dark, like a short-term memory trigger.</t>
+  </si>
+  <si>
+    <t>• Memory Bloo</t>
+  </si>
+  <si>
+    <t>• Resonant Bloom</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +461,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -469,7 +469,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -482,26 +482,26 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added moodlight-quartet and updated readme tables
</commit_message>
<xml_diff>
--- a/docs/essence-originals-projects.xlsx
+++ b/docs/essence-originals-projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\electric-essence\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C10AC78-D2D3-4E99-9BED-941BBD92DFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A2853C-ECB4-4D20-B535-C4B7FAB9F74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{C837B0F8-5954-4C5E-A065-EBAD09D629A6}"/>
+    <workbookView xWindow="38280" yWindow="3525" windowWidth="29040" windowHeight="15840" xr2:uid="{C837B0F8-5954-4C5E-A065-EBAD09D629A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Project</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>• Resonant Bloom</t>
+  </si>
+  <si>
+    <t>Moodlight Quartet</t>
+  </si>
+  <si>
+    <t>An RGB LED that reacts to light and motion in four different ways.</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DD60BD-FCD3-4516-9D8A-F004C947FC08}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,6 +510,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>